<commit_message>
CAN Traffic Analysis table - moved from wiki to this file
</commit_message>
<xml_diff>
--- a/S73 CAN Traffic Analysis.xlsx
+++ b/S73 CAN Traffic Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\50534259\Dropbox\eBike\Super 73 R\modbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353FB643-D7AE-432F-AE77-2CC8C64012BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CDE85C-D696-452A-B663-3464B2DE49D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="MSG Spec" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
     <author>Smith, Paul</author>
   </authors>
   <commentList>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{486A0013-2184-42A8-AD21-B8986A9DA2E1}">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{486A0013-2184-42A8-AD21-B8986A9DA2E1}">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{B64C16AB-AC94-4FDD-92A2-AE0BE462A3FC}">
+    <comment ref="M5" authorId="0" shapeId="0" xr:uid="{B64C16AB-AC94-4FDD-92A2-AE0BE462A3FC}">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="206">
   <si>
     <t>ID</t>
   </si>
@@ -330,12 +330,6 @@
   </si>
   <si>
     <t>Speed, Brake, ...</t>
-  </si>
-  <si>
-    <t>Speed LSB (00-FF)</t>
-  </si>
-  <si>
-    <t>Speed MSB (00-04?)</t>
   </si>
   <si>
     <t>Brake (60/64)</t>
@@ -689,6 +683,39 @@
   </si>
   <si>
     <t>Controller reads throttle position at startup and uses this as Min Throttle to calibrate throttle %.</t>
+  </si>
+  <si>
+    <t>Super73 CAN Traffic Analysis</t>
+  </si>
+  <si>
+    <t>Conventions:</t>
+  </si>
+  <si>
+    <t>D2,D1 : a 16-bit value little endian</t>
+  </si>
+  <si>
+    <t>D5/b3 : 3rd bit (from little end) of D5</t>
+  </si>
+  <si>
+    <t>Speed MSB (00-0F)</t>
+  </si>
+  <si>
+    <t>Speed LSB (00-FE, even #s only)</t>
+  </si>
+  <si>
+    <t>uint(15b)</t>
+  </si>
+  <si>
+    <t>range remaining?</t>
+  </si>
+  <si>
+    <t>Stays all zeros (except H7=0x10) when not moving.  Other bytes go non-zero while throttle pressed.. Maybe torque, current flow?  Go back to zero when off throttle, even when in motion (coasting)</t>
+  </si>
+  <si>
+    <t>(power/torque related data maybe?  Zeros when at rest or coasting, non-zeros when driving under power.</t>
+  </si>
+  <si>
+    <t>Ctrl?</t>
   </si>
 </sst>
 </file>
@@ -772,7 +799,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -804,6 +831,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1101,9 +1131,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC40B2B-00BA-4645-9F63-365F311F9F0B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:Y27"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1112,269 +1144,139 @@
     <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="11.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="10.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="11.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="12" width="10.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="14.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="8.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="14" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="17" max="23" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="12" width="10.140625" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="8.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="14" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="23" width="16.140625" customWidth="1"/>
     <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="59.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:25" ht="33" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="33" x14ac:dyDescent="0.3">
+      <c r="B5" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D5" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E5" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G5" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="K5" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="N2" s="13" t="s">
+      <c r="L5" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="M5" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="O5" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P5" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="R5" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="S5" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="T5" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="U5" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="V5" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="W2" s="12" t="s">
+      <c r="W5" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="X5" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="Y2" s="13" t="s">
+      <c r="Y5" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="14">
-        <v>200</v>
-      </c>
-      <c r="D3" s="14">
-        <v>8</v>
-      </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-    </row>
-    <row r="4" spans="2:25" ht="33" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="14">
-        <v>201</v>
-      </c>
-      <c r="D4" s="14">
-        <v>5</v>
-      </c>
-      <c r="E4" s="14">
-        <v>100</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q4" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-    </row>
-    <row r="5" spans="2:25" ht="33" x14ac:dyDescent="0.25">
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14">
-        <v>5</v>
-      </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="K5" s="14">
-        <v>0</v>
-      </c>
-      <c r="L5" s="14">
-        <v>1</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-    </row>
-    <row r="6" spans="2:25" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>76</v>
       </c>
       <c r="C6" s="14">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D6" s="14">
         <v>8</v>
       </c>
-      <c r="E6" s="14">
-        <v>1000</v>
-      </c>
+      <c r="E6" s="14"/>
       <c r="F6" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>180</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
       <c r="I6" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>170</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
-      <c r="O6" s="14" t="s">
-        <v>171</v>
-      </c>
+      <c r="O6" s="14"/>
       <c r="P6" s="14"/>
-      <c r="Q6" s="14" t="s">
-        <v>82</v>
-      </c>
+      <c r="Q6" s="14"/>
       <c r="R6" s="14"/>
       <c r="S6" s="14"/>
       <c r="T6" s="14"/>
@@ -1384,135 +1286,144 @@
       <c r="X6" s="14"/>
       <c r="Y6" s="14"/>
     </row>
-    <row r="7" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="49.5" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C7" s="14">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D7" s="14">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E7" s="14">
-        <v>31835</v>
+        <v>100</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
+        <v>78</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>163</v>
+      </c>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
+      <c r="P7" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>199</v>
+      </c>
       <c r="R7" s="14"/>
       <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
       <c r="U7" s="14"/>
       <c r="V7" s="14"/>
       <c r="W7" s="14"/>
       <c r="X7" s="14"/>
-      <c r="Y7" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="14">
-        <v>210</v>
-      </c>
+      <c r="Y7" s="14"/>
+    </row>
+    <row r="8" spans="1:25" ht="33" x14ac:dyDescent="0.25">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="14">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E8" s="14"/>
-      <c r="F8" s="14" t="s">
-        <v>86</v>
-      </c>
+      <c r="F8" s="14"/>
       <c r="G8" s="14" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
+        <v>164</v>
+      </c>
+      <c r="K8" s="14">
+        <v>0</v>
+      </c>
+      <c r="L8" s="14">
+        <v>1</v>
+      </c>
       <c r="M8" s="14" t="s">
-        <v>75</v>
+        <v>180</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
-      <c r="P8" s="14">
-        <v>53</v>
-      </c>
-      <c r="Q8" s="14">
-        <v>37</v>
-      </c>
-      <c r="R8" s="14">
-        <v>33</v>
-      </c>
-      <c r="S8" s="14">
-        <v>52</v>
-      </c>
-      <c r="T8" s="14">
-        <v>58</v>
-      </c>
-      <c r="U8" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="V8" s="14">
-        <v>32</v>
-      </c>
-      <c r="W8" s="14">
-        <v>30</v>
-      </c>
-      <c r="X8" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y8" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+    </row>
+    <row r="9" spans="1:25" ht="49.5" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C9" s="14">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D9" s="14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E9" s="14">
-        <v>31836</v>
+        <v>1000</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
+        <v>34</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>168</v>
+      </c>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
+      <c r="O9" s="14" t="s">
+        <v>169</v>
+      </c>
       <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
+      <c r="Q9" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="R9" s="14"/>
       <c r="S9" s="14"/>
       <c r="T9" s="14"/>
@@ -1520,89 +1431,65 @@
       <c r="V9" s="14"/>
       <c r="W9" s="14"/>
       <c r="X9" s="14"/>
-      <c r="Y9" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="2:25" ht="33" x14ac:dyDescent="0.25">
+      <c r="Y9" s="14"/>
+    </row>
+    <row r="10" spans="1:25" ht="66" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="14">
-        <v>211</v>
+        <v>205</v>
+      </c>
+      <c r="C10" s="16">
+        <v>203</v>
       </c>
       <c r="D10" s="14">
         <v>8</v>
       </c>
-      <c r="E10" s="14"/>
+      <c r="E10" s="14">
+        <v>100</v>
+      </c>
       <c r="F10" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="G10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>173</v>
-      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
-      <c r="M10" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="M10" s="14"/>
       <c r="N10" s="14"/>
       <c r="O10" s="14"/>
-      <c r="P10" s="14">
-        <v>30</v>
-      </c>
-      <c r="Q10" s="14">
-        <v>36</v>
-      </c>
-      <c r="R10" s="14">
-        <v>30</v>
-      </c>
-      <c r="S10" s="14">
-        <v>33</v>
-      </c>
-      <c r="T10" s="14">
-        <v>30</v>
-      </c>
-      <c r="U10" s="14">
-        <v>31</v>
-      </c>
-      <c r="V10" s="14">
-        <v>30</v>
-      </c>
-      <c r="W10" s="14">
-        <v>36</v>
-      </c>
-      <c r="X10" s="14">
-        <v>6030106</v>
-      </c>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
       <c r="Y10" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C11" s="14">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D11" s="14">
         <v>0</v>
       </c>
       <c r="E11" s="14">
-        <v>22121</v>
+        <v>31835</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -1623,173 +1510,191 @@
       <c r="W11" s="14"/>
       <c r="X11" s="14"/>
       <c r="Y11" s="14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="2:25" ht="33" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>76</v>
       </c>
       <c r="C12" s="14">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="D12" s="14">
         <v>8</v>
       </c>
-      <c r="E12" s="14">
-        <v>50</v>
-      </c>
+      <c r="E12" s="14"/>
       <c r="F12" s="14" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="L12" s="14" t="s">
-        <v>189</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
       <c r="M12" s="14" t="s">
-        <v>194</v>
+        <v>75</v>
       </c>
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
-      <c r="P12" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q12" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
+      <c r="P12" s="14">
+        <v>53</v>
+      </c>
+      <c r="Q12" s="14">
+        <v>37</v>
+      </c>
+      <c r="R12" s="14">
+        <v>33</v>
+      </c>
+      <c r="S12" s="14">
+        <v>52</v>
+      </c>
+      <c r="T12" s="14">
+        <v>58</v>
+      </c>
+      <c r="U12" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="V12" s="14">
+        <v>32</v>
+      </c>
+      <c r="W12" s="14">
+        <v>30</v>
+      </c>
+      <c r="X12" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="Y12" s="14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" spans="2:25" ht="49.5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C13" s="14">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="D13" s="14">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E13" s="14">
-        <v>50</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="K13" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="L13" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="M13" s="14" t="s">
-        <v>195</v>
-      </c>
+        <v>31836</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
-      <c r="R13" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="S13" s="14" t="s">
-        <v>186</v>
-      </c>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
       <c r="T13" s="14"/>
       <c r="U13" s="14"/>
       <c r="V13" s="14"/>
       <c r="W13" s="14"/>
       <c r="X13" s="14"/>
       <c r="Y13" s="14" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="14" spans="2:25" ht="49.5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="33" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C14" s="14">
-        <v>300</v>
+        <v>211</v>
       </c>
       <c r="D14" s="14">
         <v>8</v>
       </c>
-      <c r="E14" s="14">
-        <v>100</v>
-      </c>
+      <c r="E14" s="14"/>
       <c r="F14" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+        <v>34</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>171</v>
+      </c>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
+      <c r="M14" s="14" t="s">
+        <v>75</v>
+      </c>
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
-      <c r="P14" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-    </row>
-    <row r="15" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="P14" s="14">
+        <v>30</v>
+      </c>
+      <c r="Q14" s="14">
+        <v>36</v>
+      </c>
+      <c r="R14" s="14">
+        <v>30</v>
+      </c>
+      <c r="S14" s="14">
+        <v>33</v>
+      </c>
+      <c r="T14" s="14">
+        <v>30</v>
+      </c>
+      <c r="U14" s="14">
+        <v>31</v>
+      </c>
+      <c r="V14" s="14">
+        <v>30</v>
+      </c>
+      <c r="W14" s="14">
+        <v>36</v>
+      </c>
+      <c r="X14" s="14">
+        <v>6030106</v>
+      </c>
+      <c r="Y14" s="14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C15" s="14">
-        <v>302</v>
+        <v>212</v>
       </c>
       <c r="D15" s="14">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E15" s="14">
-        <v>31834</v>
-      </c>
-      <c r="F15" s="14"/>
+        <v>22121</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>91</v>
+      </c>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -1799,138 +1704,142 @@
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
-      <c r="P15" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="14">
-        <v>0</v>
-      </c>
-      <c r="R15" s="14">
-        <v>0</v>
-      </c>
-      <c r="S15" s="14">
-        <v>0</v>
-      </c>
-      <c r="T15" s="14">
-        <v>0</v>
-      </c>
-      <c r="U15" s="14">
-        <v>0</v>
-      </c>
-      <c r="V15" s="14">
-        <v>0</v>
-      </c>
-      <c r="W15" s="14">
-        <v>0</v>
-      </c>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
       <c r="X15" s="14"/>
-      <c r="Y15" s="14"/>
-    </row>
-    <row r="16" spans="2:25" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C16" s="15">
-        <v>400</v>
-      </c>
-      <c r="D16" s="15">
-        <v>8</v>
-      </c>
-      <c r="E16" s="15">
-        <v>107</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
+      <c r="Y15" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="33" x14ac:dyDescent="0.25">
+      <c r="B16" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="14">
+        <v>222</v>
+      </c>
+      <c r="D16" s="14">
+        <v>8</v>
+      </c>
+      <c r="E16" s="14">
+        <v>50</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>192</v>
+      </c>
       <c r="N16" s="14"/>
       <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="S16" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="T16" s="14" t="s">
-        <v>104</v>
-      </c>
+      <c r="P16" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q16" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="T16" s="14"/>
       <c r="U16" s="14"/>
       <c r="V16" s="14"/>
       <c r="W16" s="14"/>
       <c r="X16" s="14"/>
       <c r="Y16" s="14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="2:25" ht="49.5" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C17" s="14">
-        <v>401</v>
+        <v>222</v>
       </c>
       <c r="D17" s="14">
         <v>8</v>
       </c>
       <c r="E17" s="14">
-        <v>106</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
+        <v>50</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>193</v>
+      </c>
       <c r="N17" s="14"/>
       <c r="O17" s="14"/>
-      <c r="P17" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q17" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="U17" s="14" t="s">
-        <v>110</v>
-      </c>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="S17" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
       <c r="V17" s="14"/>
       <c r="W17" s="14"/>
       <c r="X17" s="14"/>
       <c r="Y17" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="2:25" ht="33" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="2:25" ht="49.5" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="C18" s="14">
-        <v>402</v>
+        <v>300</v>
       </c>
       <c r="D18" s="14">
         <v>8</v>
       </c>
       <c r="E18" s="14">
-        <v>3183</v>
+        <v>100</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
@@ -1942,38 +1851,34 @@
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
       <c r="P18" s="14" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
+      <c r="R18" s="14" t="s">
+        <v>98</v>
+      </c>
       <c r="S18" s="14"/>
       <c r="T18" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="U18" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="V18" s="14" t="s">
-        <v>116</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
       <c r="W18" s="14"/>
       <c r="X18" s="14"/>
-      <c r="Y18" s="14" t="s">
-        <v>117</v>
-      </c>
+      <c r="Y18" s="14"/>
     </row>
     <row r="19" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="C19" s="14">
-        <v>403</v>
+        <v>302</v>
       </c>
       <c r="D19" s="14">
         <v>8</v>
       </c>
       <c r="E19" s="14">
-        <v>3184</v>
+        <v>31834</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
@@ -1985,40 +1890,48 @@
       <c r="M19" s="14"/>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="U19" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="V19" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="W19" s="14"/>
+      <c r="P19" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="14">
+        <v>0</v>
+      </c>
+      <c r="R19" s="14">
+        <v>0</v>
+      </c>
+      <c r="S19" s="14">
+        <v>0</v>
+      </c>
+      <c r="T19" s="14">
+        <v>0</v>
+      </c>
+      <c r="U19" s="14">
+        <v>0</v>
+      </c>
+      <c r="V19" s="14">
+        <v>0</v>
+      </c>
+      <c r="W19" s="14">
+        <v>0</v>
+      </c>
       <c r="X19" s="14"/>
-      <c r="Y19" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="14">
-        <v>404</v>
-      </c>
-      <c r="D20" s="14">
-        <v>8</v>
-      </c>
-      <c r="E20" s="14">
-        <v>3183</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>122</v>
+      <c r="Y19" s="14"/>
+    </row>
+    <row r="20" spans="2:25" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="15">
+        <v>400</v>
+      </c>
+      <c r="D20" s="15">
+        <v>8</v>
+      </c>
+      <c r="E20" s="15">
+        <v>107</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -2032,35 +1945,37 @@
       <c r="P20" s="14"/>
       <c r="Q20" s="14"/>
       <c r="R20" s="14" t="s">
-        <v>123</v>
+        <v>181</v>
       </c>
       <c r="S20" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="T20" s="14"/>
+        <v>182</v>
+      </c>
+      <c r="T20" s="14" t="s">
+        <v>102</v>
+      </c>
       <c r="U20" s="14"/>
       <c r="V20" s="14"/>
       <c r="W20" s="14"/>
       <c r="X20" s="14"/>
       <c r="Y20" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="2:25" ht="49.5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C21" s="14">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="D21" s="14">
         <v>8</v>
       </c>
       <c r="E21" s="14">
-        <v>4249</v>
+        <v>106</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
@@ -2072,51 +1987,41 @@
       <c r="N21" s="14"/>
       <c r="O21" s="14"/>
       <c r="P21" s="14" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="Q21" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="R21" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="S21" s="14" t="s">
-        <v>130</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
       <c r="T21" s="14" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="U21" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="V21" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="W21" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="X21" s="14" t="s">
-        <v>135</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="V21" s="14"/>
+      <c r="W21" s="14"/>
+      <c r="X21" s="14"/>
       <c r="Y21" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="2:25" ht="49.5" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25" ht="33" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C22" s="14">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="D22" s="14">
         <v>8</v>
       </c>
       <c r="E22" s="14">
-        <v>30491</v>
+        <v>3183</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -2128,52 +2033,40 @@
       <c r="N22" s="14"/>
       <c r="O22" s="14"/>
       <c r="P22" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q22" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="R22" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="S22" s="14" t="s">
-        <v>141</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
       <c r="T22" s="14" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="U22" s="14" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="V22" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="W22" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="X22" s="14" t="s">
-        <v>145</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="W22" s="14"/>
+      <c r="X22" s="14"/>
       <c r="Y22" s="14" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C23" s="14">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="D23" s="14">
         <v>8</v>
       </c>
       <c r="E23" s="14">
-        <v>4247</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>147</v>
-      </c>
+        <v>3184</v>
+      </c>
+      <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
@@ -2183,48 +2076,40 @@
       <c r="M23" s="14"/>
       <c r="N23" s="14"/>
       <c r="O23" s="14"/>
-      <c r="P23" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="14">
-        <v>0</v>
-      </c>
-      <c r="R23" s="14">
-        <v>0</v>
-      </c>
-      <c r="S23" s="14">
-        <v>0</v>
-      </c>
-      <c r="T23" s="14">
-        <v>0</v>
-      </c>
-      <c r="U23" s="14">
-        <v>0</v>
-      </c>
-      <c r="V23" s="14">
-        <v>0</v>
-      </c>
-      <c r="W23" s="14">
-        <v>0</v>
-      </c>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="U23" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="V23" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="W23" s="14"/>
       <c r="X23" s="14"/>
-      <c r="Y23" s="14"/>
-    </row>
-    <row r="24" spans="2:25" ht="33" x14ac:dyDescent="0.25">
+      <c r="Y23" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C24" s="14">
-        <v>423</v>
+        <v>404</v>
       </c>
       <c r="D24" s="14">
         <v>8</v>
       </c>
       <c r="E24" s="14">
-        <v>0</v>
+        <v>3183</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
@@ -2235,50 +2120,38 @@
       <c r="M24" s="14"/>
       <c r="N24" s="14"/>
       <c r="O24" s="14"/>
-      <c r="P24" s="14">
-        <v>88</v>
-      </c>
-      <c r="Q24" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="R24" s="14">
-        <v>88</v>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14" t="s">
+        <v>121</v>
       </c>
       <c r="S24" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="T24" s="14">
-        <v>88</v>
-      </c>
-      <c r="U24" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="V24" s="14">
-        <v>88</v>
-      </c>
-      <c r="W24" s="14" t="s">
-        <v>149</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="T24" s="14"/>
+      <c r="U24" s="14"/>
+      <c r="V24" s="14"/>
+      <c r="W24" s="14"/>
       <c r="X24" s="14"/>
       <c r="Y24" s="14" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="25" spans="2:25" ht="33" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="2:25" ht="49.5" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="C25" s="14">
-        <v>466</v>
+        <v>410</v>
       </c>
       <c r="D25" s="14">
         <v>8</v>
       </c>
       <c r="E25" s="14">
-        <v>2124</v>
+        <v>4249</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
@@ -2289,50 +2162,52 @@
       <c r="M25" s="14"/>
       <c r="N25" s="14"/>
       <c r="O25" s="14"/>
-      <c r="P25" s="14">
-        <v>30</v>
-      </c>
-      <c r="Q25" s="14">
-        <v>32</v>
-      </c>
-      <c r="R25" s="14">
-        <v>30</v>
-      </c>
-      <c r="S25" s="14">
-        <v>35</v>
-      </c>
-      <c r="T25" s="14">
-        <v>56</v>
-      </c>
-      <c r="U25" s="14">
-        <v>35</v>
-      </c>
-      <c r="V25" s="14">
-        <v>30</v>
-      </c>
-      <c r="W25" s="14">
-        <v>31</v>
+      <c r="P25" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q25" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="R25" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="S25" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="T25" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="U25" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="V25" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="W25" s="14" t="s">
+        <v>132</v>
       </c>
       <c r="X25" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="Y25" s="14"/>
-    </row>
-    <row r="26" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="Y25" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="2:25" ht="49.5" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
-        <v>154</v>
+        <v>100</v>
       </c>
       <c r="C26" s="14">
-        <v>466</v>
+        <v>411</v>
       </c>
       <c r="D26" s="14">
         <v>8</v>
       </c>
       <c r="E26" s="14">
-        <v>2124</v>
+        <v>30491</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
@@ -2343,50 +2218,52 @@
       <c r="M26" s="14"/>
       <c r="N26" s="14"/>
       <c r="O26" s="14"/>
-      <c r="P26" s="14">
-        <v>0</v>
+      <c r="P26" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="Q26" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="R26" s="14">
-        <v>0</v>
-      </c>
-      <c r="S26" s="14">
-        <v>0</v>
-      </c>
-      <c r="T26" s="14">
-        <v>0</v>
-      </c>
-      <c r="U26" s="14">
-        <v>33</v>
-      </c>
-      <c r="V26" s="14">
-        <v>30</v>
-      </c>
-      <c r="W26" s="14">
-        <v>30</v>
+        <v>137</v>
+      </c>
+      <c r="R26" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="S26" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="T26" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="U26" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="V26" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="W26" s="14" t="s">
+        <v>125</v>
       </c>
       <c r="X26" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="Y26" s="14"/>
-    </row>
-    <row r="27" spans="2:25" ht="33" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="Y26" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>17</v>
+        <v>100</v>
+      </c>
+      <c r="C27" s="14">
+        <v>412</v>
       </c>
       <c r="D27" s="14">
         <v>8</v>
       </c>
       <c r="E27" s="14">
-        <v>100</v>
+        <v>4247</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
@@ -2397,28 +2274,242 @@
       <c r="M27" s="14"/>
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="U27" s="14"/>
-      <c r="V27" s="14"/>
-      <c r="W27" s="14"/>
+      <c r="P27" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="14">
+        <v>0</v>
+      </c>
+      <c r="R27" s="14">
+        <v>0</v>
+      </c>
+      <c r="S27" s="14">
+        <v>0</v>
+      </c>
+      <c r="T27" s="14">
+        <v>0</v>
+      </c>
+      <c r="U27" s="14">
+        <v>0</v>
+      </c>
+      <c r="V27" s="14">
+        <v>0</v>
+      </c>
+      <c r="W27" s="14">
+        <v>0</v>
+      </c>
       <c r="X27" s="14"/>
       <c r="Y27" s="14"/>
     </row>
+    <row r="28" spans="2:25" ht="33" x14ac:dyDescent="0.25">
+      <c r="B28" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="14">
+        <v>423</v>
+      </c>
+      <c r="D28" s="14">
+        <v>8</v>
+      </c>
+      <c r="E28" s="14">
+        <v>0</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14">
+        <v>88</v>
+      </c>
+      <c r="Q28" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="R28" s="14">
+        <v>88</v>
+      </c>
+      <c r="S28" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="T28" s="14">
+        <v>88</v>
+      </c>
+      <c r="U28" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="V28" s="14">
+        <v>88</v>
+      </c>
+      <c r="W28" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="X28" s="14"/>
+      <c r="Y28" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="2:25" ht="33" x14ac:dyDescent="0.25">
+      <c r="B29" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" s="14">
+        <v>466</v>
+      </c>
+      <c r="D29" s="14">
+        <v>8</v>
+      </c>
+      <c r="E29" s="14">
+        <v>2124</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="14">
+        <v>30</v>
+      </c>
+      <c r="Q29" s="14">
+        <v>32</v>
+      </c>
+      <c r="R29" s="14">
+        <v>30</v>
+      </c>
+      <c r="S29" s="14">
+        <v>35</v>
+      </c>
+      <c r="T29" s="14">
+        <v>56</v>
+      </c>
+      <c r="U29" s="14">
+        <v>35</v>
+      </c>
+      <c r="V29" s="14">
+        <v>30</v>
+      </c>
+      <c r="W29" s="14">
+        <v>31</v>
+      </c>
+      <c r="X29" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y29" s="14"/>
+    </row>
+    <row r="30" spans="2:25" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B30" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="14">
+        <v>466</v>
+      </c>
+      <c r="D30" s="14">
+        <v>8</v>
+      </c>
+      <c r="E30" s="14">
+        <v>2124</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="R30" s="14">
+        <v>0</v>
+      </c>
+      <c r="S30" s="14">
+        <v>0</v>
+      </c>
+      <c r="T30" s="14">
+        <v>0</v>
+      </c>
+      <c r="U30" s="14">
+        <v>33</v>
+      </c>
+      <c r="V30" s="14">
+        <v>30</v>
+      </c>
+      <c r="W30" s="14">
+        <v>30</v>
+      </c>
+      <c r="X30" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y30" s="14"/>
+    </row>
+    <row r="31" spans="2:25" ht="33" x14ac:dyDescent="0.25">
+      <c r="B31" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="14">
+        <v>8</v>
+      </c>
+      <c r="E31" s="14">
+        <v>100</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="U31" s="14"/>
+      <c r="V31" s="14"/>
+      <c r="W31" s="14"/>
+      <c r="X31" s="14"/>
+      <c r="Y31" s="14"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="P4:S5 U4:W5 P6:W11 P14:W27 P12:Q13 T12:W13">
+  <conditionalFormatting sqref="P7:S8 U7:W8 P9:W15 P18:W31 P16:Q17 T16:W17">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>COLUMN(P4)-COLUMN($P4)+1&gt;$D4</formula>
+      <formula>COLUMN(P7)-COLUMN($P7)+1&gt;$D7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T5 R13:S13">
+  <conditionalFormatting sqref="T8 R17:S17">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>COLUMN(R5)-COLUMN($P4)+1&gt;$D4</formula>
+      <formula>COLUMN(R8)-COLUMN($P7)+1&gt;$D7</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>